<commit_message>
Commit on dated 28-06-2018
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18792" windowHeight="3876" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18792" windowHeight="3876" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="250">
   <si>
     <t>UserName</t>
   </si>
@@ -754,6 +754,21 @@
   </si>
   <si>
     <t xml:space="preserve"> //*[@id="mgt_fees_data_table"]/tbody/tr[last()]/td</t>
+  </si>
+  <si>
+    <t>DoubleClick Reports</t>
+  </si>
+  <si>
+    <t>ApplyFeesfromcodes</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1302,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,9 +1647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3:I60"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3383,7 +3398,7 @@
         <v>214</v>
       </c>
       <c r="I61" t="s">
-        <v>218</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3394,29 +3409,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.21875" customWidth="1"/>
     <col min="4" max="4" width="29.44140625" customWidth="1"/>
     <col min="5" max="8" width="15.5546875" customWidth="1"/>
     <col min="9" max="9" width="29.6640625" customWidth="1"/>
     <col min="10" max="10" width="31.21875" customWidth="1"/>
-    <col min="11" max="11" width="29.21875" customWidth="1"/>
-    <col min="12" max="12" width="31.109375" customWidth="1"/>
-    <col min="13" max="13" width="46" customWidth="1"/>
-    <col min="14" max="14" width="51.5546875" customWidth="1"/>
-    <col min="15" max="15" width="27.88671875" customWidth="1"/>
-    <col min="16" max="16" width="22.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="25" customWidth="1"/>
+    <col min="11" max="12" width="29.21875" customWidth="1"/>
+    <col min="13" max="13" width="31.109375" customWidth="1"/>
+    <col min="14" max="14" width="46" customWidth="1"/>
+    <col min="15" max="15" width="51.5546875" customWidth="1"/>
+    <col min="16" max="16" width="27.88671875" customWidth="1"/>
+    <col min="17" max="17" width="22.88671875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>242</v>
       </c>
@@ -3451,25 +3467,31 @@
         <v>231</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S1" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>240</v>
       </c>
@@ -3477,7 +3499,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
         <v>221</v>
@@ -3504,25 +3526,31 @@
         <v>51</v>
       </c>
       <c r="L2" t="s">
+        <v>218</v>
+      </c>
+      <c r="M2" t="s">
         <v>225</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>235</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>239</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>237</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>241</v>
       </c>
-      <c r="Q2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>240</v>
       </c>
@@ -3530,7 +3558,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="D3" t="s">
         <v>221</v>
@@ -3557,20 +3585,26 @@
         <v>51</v>
       </c>
       <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s">
         <v>234</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>236</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>244</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>238</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" t="s">
-        <v>218</v>
+      <c r="Q3" s="3"/>
+      <c r="R3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>